<commit_message>
new variant data format
</commit_message>
<xml_diff>
--- a/data/raw-load-data.xlsx
+++ b/data/raw-load-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metcmn-my.sharepoint.com/personal/steve_balogh_metc_state_mn_us/Documents/DATA/XLS/1-SARS-CoV-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AsmusAL\Documents\MetC_Locals\MTS\covid-poops\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96EDB2F5-46A7-49FB-B6E9-7663AAA1AFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D6F9307-49B2-4690-8FE3-96044314189D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21090" windowHeight="13515" xr2:uid="{AE8A8B14-72F9-4ACE-AA9E-00D9E18E4A26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AE8A8B14-72F9-4ACE-AA9E-00D9E18E4A26}"/>
   </bookViews>
   <sheets>
     <sheet name="MCES" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="567">
   <si>
     <t>save to OneDrive to update!</t>
   </si>
@@ -1711,6 +1714,30 @@
   </si>
   <si>
     <t>1076</t>
+  </si>
+  <si>
+    <t>1154</t>
+  </si>
+  <si>
+    <t>1155</t>
+  </si>
+  <si>
+    <t>1166</t>
+  </si>
+  <si>
+    <t>1167</t>
+  </si>
+  <si>
+    <t>1171</t>
+  </si>
+  <si>
+    <t>1172</t>
+  </si>
+  <si>
+    <t>1186</t>
+  </si>
+  <si>
+    <t>1187</t>
   </si>
 </sst>
 </file>
@@ -9713,13 +9740,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6D67CB-9292-41F3-90B2-AF9620A42692}">
-  <dimension ref="A1:T860"/>
+  <dimension ref="A1:T868"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B837" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B849" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A847" sqref="A847:XFD849"/>
+      <selection pane="bottomRight" activeCell="R855" sqref="R855"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -51519,6 +51546,374 @@
       <c r="N860" s="14"/>
       <c r="O860" s="14"/>
       <c r="P860" s="29"/>
+    </row>
+    <row r="861" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A861" s="28" t="s">
+        <v>559</v>
+      </c>
+      <c r="B861" s="7">
+        <v>169.68178710937499</v>
+      </c>
+      <c r="C861" s="7">
+        <v>218.19587402343799</v>
+      </c>
+      <c r="D861" s="8">
+        <v>44575</v>
+      </c>
+      <c r="E861" s="9">
+        <v>44576</v>
+      </c>
+      <c r="F861" s="10">
+        <v>1696817.87109375</v>
+      </c>
+      <c r="G861" s="10">
+        <v>2181958.7402343801</v>
+      </c>
+      <c r="H861" s="10">
+        <v>1939388.3056640651</v>
+      </c>
+      <c r="I861" s="11">
+        <v>44575</v>
+      </c>
+      <c r="J861" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K861" s="13">
+        <v>151.96496582031301</v>
+      </c>
+      <c r="L861" s="10">
+        <v>1811001.4953613295</v>
+      </c>
+      <c r="M861" s="14">
+        <v>1115511708649968.4</v>
+      </c>
+      <c r="N861" s="14">
+        <v>1041665233598710</v>
+      </c>
+      <c r="O861" s="14">
+        <v>534187299.28138977</v>
+      </c>
+      <c r="P861" s="29">
+        <v>534.18729928138976</v>
+      </c>
+    </row>
+    <row r="862" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A862" s="28" t="s">
+        <v>560</v>
+      </c>
+      <c r="B862" s="7">
+        <v>138.0165283203126</v>
+      </c>
+      <c r="C862" s="7">
+        <v>198.50640869140619</v>
+      </c>
+      <c r="D862" s="8">
+        <v>44575</v>
+      </c>
+      <c r="E862" s="9">
+        <v>44576</v>
+      </c>
+      <c r="F862" s="10">
+        <v>1380165.2832031259</v>
+      </c>
+      <c r="G862" s="10">
+        <v>1985064.086914062</v>
+      </c>
+      <c r="H862" s="10">
+        <v>1682614.685058594</v>
+      </c>
+      <c r="I862" s="11">
+        <v>44575</v>
+      </c>
+      <c r="J862" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K862" s="13">
+        <v>151.96496582031301</v>
+      </c>
+      <c r="L862" s="10"/>
+      <c r="M862" s="14">
+        <v>967818758547451.38</v>
+      </c>
+      <c r="N862" s="14"/>
+      <c r="O862" s="14"/>
+      <c r="P862" s="29"/>
+    </row>
+    <row r="863" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A863" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="B863" s="7">
+        <v>147.85991210937499</v>
+      </c>
+      <c r="C863" s="7">
+        <v>230.58364257812599</v>
+      </c>
+      <c r="D863" s="8">
+        <v>44576</v>
+      </c>
+      <c r="E863" s="9">
+        <v>44577</v>
+      </c>
+      <c r="F863" s="10">
+        <v>1478599.12109375</v>
+      </c>
+      <c r="G863" s="10">
+        <v>2305836.4257812598</v>
+      </c>
+      <c r="H863" s="10">
+        <v>1892217.7734375049</v>
+      </c>
+      <c r="I863" s="11">
+        <v>44576</v>
+      </c>
+      <c r="J863" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K863" s="13">
+        <v>148.80323791503901</v>
+      </c>
+      <c r="L863" s="10">
+        <v>1836735.8093261728</v>
+      </c>
+      <c r="M863" s="14">
+        <v>1065735377833050</v>
+      </c>
+      <c r="N863" s="14">
+        <v>1034486811830156.6</v>
+      </c>
+      <c r="O863" s="14">
+        <v>530506057.34879827</v>
+      </c>
+      <c r="P863" s="29">
+        <v>530.50605734879832</v>
+      </c>
+    </row>
+    <row r="864" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A864" s="28" t="s">
+        <v>562</v>
+      </c>
+      <c r="B864" s="7">
+        <v>155.1081665039062</v>
+      </c>
+      <c r="C864" s="7">
+        <v>201.14260253906201</v>
+      </c>
+      <c r="D864" s="8">
+        <v>44576</v>
+      </c>
+      <c r="E864" s="9">
+        <v>44577</v>
+      </c>
+      <c r="F864" s="10">
+        <v>1551081.665039062</v>
+      </c>
+      <c r="G864" s="10">
+        <v>2011426.0253906201</v>
+      </c>
+      <c r="H864" s="10">
+        <v>1781253.845214841</v>
+      </c>
+      <c r="I864" s="11">
+        <v>44576</v>
+      </c>
+      <c r="J864" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K864" s="13">
+        <v>148.80323791503901</v>
+      </c>
+      <c r="L864" s="10"/>
+      <c r="M864" s="14">
+        <v>1003238245827263</v>
+      </c>
+      <c r="N864" s="14"/>
+      <c r="O864" s="14"/>
+      <c r="P864" s="29"/>
+    </row>
+    <row r="865" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A865" s="28" t="s">
+        <v>563</v>
+      </c>
+      <c r="B865" s="7">
+        <v>112.28941650390621</v>
+      </c>
+      <c r="C865" s="7">
+        <v>175.70135498046881</v>
+      </c>
+      <c r="D865" s="8">
+        <v>44577</v>
+      </c>
+      <c r="E865" s="9">
+        <v>44578</v>
+      </c>
+      <c r="F865" s="10">
+        <v>1122894.165039062</v>
+      </c>
+      <c r="G865" s="10">
+        <v>1757013.549804688</v>
+      </c>
+      <c r="H865" s="10">
+        <v>1439953.857421875</v>
+      </c>
+      <c r="I865" s="11">
+        <v>44577</v>
+      </c>
+      <c r="J865" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K865" s="13">
+        <v>149.39880371093801</v>
+      </c>
+      <c r="L865" s="10">
+        <v>1369780.5786132815</v>
+      </c>
+      <c r="M865" s="14">
+        <v>814257147296092.38</v>
+      </c>
+      <c r="N865" s="14">
+        <v>774575949510073.25</v>
+      </c>
+      <c r="O865" s="14">
+        <v>397218435.64619142</v>
+      </c>
+      <c r="P865" s="29">
+        <v>397.21843564619144</v>
+      </c>
+    </row>
+    <row r="866" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A866" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="B866" s="7">
+        <v>109.9165771484376</v>
+      </c>
+      <c r="C866" s="7">
+        <v>150.0048828125</v>
+      </c>
+      <c r="D866" s="8">
+        <v>44577</v>
+      </c>
+      <c r="E866" s="9">
+        <v>44578</v>
+      </c>
+      <c r="F866" s="10">
+        <v>1099165.7714843759</v>
+      </c>
+      <c r="G866" s="10">
+        <v>1500048.828125</v>
+      </c>
+      <c r="H866" s="10">
+        <v>1299607.299804688</v>
+      </c>
+      <c r="I866" s="11">
+        <v>44577</v>
+      </c>
+      <c r="J866" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K866" s="13">
+        <v>149.39880371093801</v>
+      </c>
+      <c r="L866" s="10"/>
+      <c r="M866" s="14">
+        <v>734894751724054</v>
+      </c>
+      <c r="N866" s="14"/>
+      <c r="O866" s="14"/>
+      <c r="P866" s="29"/>
+    </row>
+    <row r="867" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A867" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B867" s="7">
+        <v>120.39267578125001</v>
+      </c>
+      <c r="C867" s="7">
+        <v>144.94528808593759</v>
+      </c>
+      <c r="D867" s="8">
+        <v>44578</v>
+      </c>
+      <c r="E867" s="9">
+        <v>44579</v>
+      </c>
+      <c r="F867" s="10">
+        <v>1203926.7578125</v>
+      </c>
+      <c r="G867" s="10">
+        <v>1449452.8808593759</v>
+      </c>
+      <c r="H867" s="10">
+        <v>1326689.819335938</v>
+      </c>
+      <c r="I867" s="11">
+        <v>44578</v>
+      </c>
+      <c r="J867" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K867" s="13">
+        <v>155.053634643555</v>
+      </c>
+      <c r="L867" s="10">
+        <v>1256332.2448730469</v>
+      </c>
+      <c r="M867" s="14">
+        <v>778605077246036.75</v>
+      </c>
+      <c r="N867" s="14">
+        <v>737313764159046.25</v>
+      </c>
+      <c r="O867" s="14">
+        <v>378109622.64566475</v>
+      </c>
+      <c r="P867" s="29">
+        <v>378.10962264566473</v>
+      </c>
+    </row>
+    <row r="868" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A868" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="B868" s="7">
+        <v>101.5995239257812</v>
+      </c>
+      <c r="C868" s="7">
+        <v>135.59541015625001</v>
+      </c>
+      <c r="D868" s="8">
+        <v>44578</v>
+      </c>
+      <c r="E868" s="9">
+        <v>44579</v>
+      </c>
+      <c r="F868" s="10">
+        <v>1015995.239257812</v>
+      </c>
+      <c r="G868" s="10">
+        <v>1355954.1015625</v>
+      </c>
+      <c r="H868" s="10">
+        <v>1185974.670410156</v>
+      </c>
+      <c r="I868" s="11">
+        <v>44578</v>
+      </c>
+      <c r="J868" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K868" s="13">
+        <v>155.053634643555</v>
+      </c>
+      <c r="L868" s="10"/>
+      <c r="M868" s="14">
+        <v>696022451072055.88</v>
+      </c>
+      <c r="N868" s="14"/>
+      <c r="O868" s="14"/>
+      <c r="P868" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51799,16 +52194,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14CBD8C3-82DE-4B2D-86B3-234C23B3725B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1d037e43-dc6e-49d3-a5ce-28e5ae53c4d2"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="dc302e13-f8af-4931-a923-d612bc0608e7"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>